<commit_message>
ABM Espec y Tipo Doc listos
</commit_message>
<xml_diff>
--- a/tp.xlsx
+++ b/tp.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="14">
   <si>
     <t>ABM</t>
   </si>
@@ -395,7 +395,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -474,9 +474,7 @@
       <c r="C6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="D6" s="1"/>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">

</xml_diff>

<commit_message>
Retoques a interfaz de ClubesXProfe
Solo algunos arreglitos en la parte grafica para que quedaran todos
parecidos
</commit_message>
<xml_diff>
--- a/tp.xlsx
+++ b/tp.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\Github proyectos\PAV\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="8505"/>
   </bookViews>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="26">
   <si>
     <t>ABM</t>
   </si>
@@ -99,8 +104,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -265,11 +270,19 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -311,7 +324,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -343,9 +356,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -377,6 +391,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -552,14 +567,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.42578125" customWidth="1"/>
@@ -567,7 +582,7 @@
     <col min="4" max="4" width="29.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -581,7 +596,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -593,7 +608,7 @@
       </c>
       <c r="D2" s="6"/>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
@@ -605,7 +620,7 @@
       </c>
       <c r="D3" s="6"/>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
@@ -617,7 +632,7 @@
       </c>
       <c r="D4" s="6"/>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>4</v>
       </c>
@@ -629,7 +644,7 @@
       </c>
       <c r="D5" s="6"/>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
@@ -641,7 +656,7 @@
       </c>
       <c r="D6" s="7"/>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
@@ -655,7 +670,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15.75" thickBot="1">
+    <row r="8" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
         <v>7</v>
       </c>
@@ -667,8 +682,8 @@
       </c>
       <c r="D8" s="10"/>
     </row>
-    <row r="9" spans="1:4" ht="15.75" thickBot="1"/>
-    <row r="10" spans="1:4">
+    <row r="9" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
         <v>14</v>
       </c>
@@ -682,7 +697,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
         <v>25</v>
       </c>
@@ -690,7 +705,7 @@
       <c r="C11" s="11"/>
       <c r="D11" s="18"/>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
         <v>16</v>
       </c>
@@ -698,7 +713,7 @@
       <c r="C12" s="16"/>
       <c r="D12" s="6"/>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
         <v>17</v>
       </c>
@@ -712,7 +727,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
         <v>22</v>
       </c>
@@ -720,15 +735,19 @@
       <c r="C14" s="16"/>
       <c r="D14" s="6"/>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="16"/>
-      <c r="C15" s="16"/>
+      <c r="B15" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>23</v>
+      </c>
       <c r="D15" s="6"/>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
         <v>19</v>
       </c>
@@ -736,15 +755,19 @@
       <c r="C16" s="16"/>
       <c r="D16" s="6"/>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="B17" s="16"/>
-      <c r="C17" s="16"/>
+      <c r="B17" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>23</v>
+      </c>
       <c r="D17" s="6"/>
     </row>
-    <row r="18" spans="1:4" ht="15.75" thickBot="1">
+    <row r="18" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="17" t="s">
         <v>21</v>
       </c>
@@ -756,7 +779,7 @@
       </c>
       <c r="D18" s="10"/>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="11"/>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
@@ -768,24 +791,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>